<commit_message>
Update the contents to fix errors.
</commit_message>
<xml_diff>
--- a/test/xlsx/borders/colors.xlsx
+++ b/test/xlsx/borders/colors.xlsx
@@ -36,7 +36,7 @@
   </si>
   <si>
     <t>&lt;- Yellow
-Blue-&gt;
+Purple -&gt;
 Light Blue \</t>
   </si>
 </sst>
@@ -438,12 +438,12 @@
   <dimension ref="B3:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>